<commit_message>
adding new coding analysis
</commit_message>
<xml_diff>
--- a/analysis/fullData_analysis/survey_analysis/maxqda_survey_responses.xlsx
+++ b/analysis/fullData_analysis/survey_analysis/maxqda_survey_responses.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasu1\Code\RTmocapFB\analysis\fullData_analysis\survey_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D907CF1-3A91-4B38-8E7B-3386BBD34E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E53BB9-F866-4A4E-BC7B-BEC9BF2B0920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8BC8F3FD-F082-45AC-93E5-3BB8224EB29D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{8BC8F3FD-F082-45AC-93E5-3BB8224EB29D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="all" sheetId="1" r:id="rId1"/>
+    <sheet name="open" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="186">
   <si>
     <t>Document Group</t>
   </si>
@@ -497,13 +498,298 @@
   </si>
   <si>
     <t>OE2 suggestions</t>
+  </si>
+  <si>
+    <t>Favoring SF</t>
+  </si>
+  <si>
+    <t>Favoring TF</t>
+  </si>
+  <si>
+    <t>Sub themes</t>
+  </si>
+  <si>
+    <t>Improved comprehension</t>
+  </si>
+  <si>
+    <t>Reduced error bounds more</t>
+  </si>
+  <si>
+    <t>Used to on-off response</t>
+  </si>
+  <si>
+    <t>More intuitive</t>
+  </si>
+  <si>
+    <t>Self-correction over time</t>
+  </si>
+  <si>
+    <t>Slight preference, but not significant</t>
+  </si>
+  <si>
+    <t>Main Themes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1 </t>
+  </si>
+  <si>
+    <t>Count (SF)</t>
+  </si>
+  <si>
+    <t>Count (TF)</t>
+  </si>
+  <si>
+    <t>Count (NF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less confusing </t>
+  </si>
+  <si>
+    <t>Less frustrating/ stressful</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Technically I preferred the scaled feedback, because I like the notion of an extra degree of freedom within the feedback itself</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. However, I couldn't feel its scaling during the trials itself, so perhaps the value was lost on me.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The the very short feedback vibration for minor changes gave me so much more free workload to correct my step. In direct comparison the consistent and long feedback felt a bit like an overkill.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="0.79998168889431442"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>But I do not know if I would have preferred a short consistent feedback.</t>
+    </r>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> I feel like the scaled one it is nice at first to train a bit but then the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="0.499984740745262"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>constant one get to be less emotionally (psychological) draining  once you understood the angle and you just need small adjustment .</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">although subtle, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the scaled did seem less annoying and I could see using it for longer periods of time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">it is a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>very sutil angle change</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> so the scaled doesnt help so much when adapting the position on the foot</t>
+    </r>
+  </si>
+  <si>
+    <t>Gives more specific information</t>
+  </si>
+  <si>
+    <t>Helpful, but irritating</t>
+  </si>
+  <si>
+    <t>Better over time</t>
+  </si>
+  <si>
+    <t>Subtle differences / Either works</t>
+  </si>
+  <si>
+    <t>Changes over time</t>
+  </si>
+  <si>
+    <t>Neither</t>
+  </si>
+  <si>
+    <t>Needs to fit individual needs</t>
+  </si>
+  <si>
+    <t>Less taxing</t>
+  </si>
+  <si>
+    <t>Learn more with less</t>
+  </si>
+  <si>
+    <t>Comfortable over time</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>was a bit stressed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> about performing well in the beginning and the feedback was a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bit irritating and frustrating</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. After some time, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I got used to it and it felt kind of rewarding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> even forgot about it at some point </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>when I found the right angle.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,16 +805,98 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="0.79998168889431442"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -536,11 +904,134 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -548,6 +1039,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB35C5CC-E3B2-4C71-AEDF-E9A6665F5A9A}">
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4547,4 +5107,1011 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3279C05-889A-4FA7-9B94-B3AA5CA38D51}">
+  <dimension ref="A1:L63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="46.88671875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="56.21875" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="20" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" ht="216" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>0</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>0</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>0</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="5">
+        <v>2</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>0</v>
+      </c>
+      <c r="B26" s="5">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>2</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>0</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>0</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5">
+        <v>2</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>0</v>
+      </c>
+      <c r="B32" s="5">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5">
+        <v>2</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5">
+        <v>2</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>2</v>
+      </c>
+      <c r="B34" s="5">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="5">
+        <v>2</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>2</v>
+      </c>
+      <c r="B36" s="5">
+        <v>2</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="5">
+        <v>2</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>0</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="12">
+        <v>2</v>
+      </c>
+      <c r="D41" s="12">
+        <v>1</v>
+      </c>
+      <c r="E41" s="14"/>
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
+      <c r="B42" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="12">
+        <v>2</v>
+      </c>
+      <c r="D42" s="12">
+        <v>3</v>
+      </c>
+      <c r="E42" s="14"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="13"/>
+      <c r="B43" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="12">
+        <v>2</v>
+      </c>
+      <c r="D43" s="12">
+        <v>3</v>
+      </c>
+      <c r="E43" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="15"/>
+      <c r="B45" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="12">
+        <v>3</v>
+      </c>
+      <c r="D45" s="12">
+        <v>1</v>
+      </c>
+      <c r="E45" s="14"/>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12">
+        <v>1</v>
+      </c>
+      <c r="E46" s="14"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="16"/>
+      <c r="B47" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="12">
+        <v>1</v>
+      </c>
+      <c r="D47" s="12">
+        <v>1</v>
+      </c>
+      <c r="E47" s="14"/>
+    </row>
+    <row r="48" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="17"/>
+      <c r="B48" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" s="18">
+        <v>1</v>
+      </c>
+      <c r="D48" s="18">
+        <v>1</v>
+      </c>
+      <c r="E48" s="19"/>
+    </row>
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="22"/>
+    </row>
+    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C54" s="12">
+        <v>2</v>
+      </c>
+      <c r="D54" s="12">
+        <v>4</v>
+      </c>
+      <c r="E54" s="14"/>
+    </row>
+    <row r="55" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="13"/>
+      <c r="B55" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="12">
+        <v>1</v>
+      </c>
+      <c r="D55" s="12">
+        <v>1</v>
+      </c>
+      <c r="E55" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="13"/>
+      <c r="B56" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12">
+        <v>1</v>
+      </c>
+      <c r="E56" s="14"/>
+    </row>
+    <row r="57" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" s="12">
+        <v>3</v>
+      </c>
+      <c r="D57" s="12">
+        <v>1</v>
+      </c>
+      <c r="E57" s="14"/>
+    </row>
+    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="15"/>
+      <c r="B58" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="12">
+        <v>1</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="14"/>
+    </row>
+    <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C59" s="12">
+        <v>1</v>
+      </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" s="12">
+        <v>1</v>
+      </c>
+      <c r="D60" s="12">
+        <v>1</v>
+      </c>
+      <c r="E60" s="14"/>
+    </row>
+    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="16"/>
+      <c r="B61" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="12">
+        <v>1</v>
+      </c>
+      <c r="D61" s="12">
+        <v>1</v>
+      </c>
+      <c r="E61" s="14"/>
+    </row>
+    <row r="62" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="17"/>
+      <c r="B62" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18">
+        <v>1</v>
+      </c>
+      <c r="E62" s="19"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A46:A48"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>